<commit_message>
Commited for ContactUs Page Test
</commit_message>
<xml_diff>
--- a/src/main/resources/ContactUsData.xlsx
+++ b/src/main/resources/ContactUsData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D0FFFA-808C-415A-B2EE-754B3D33AB82}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642C869B-A766-4515-8AB6-FFA0E2F9773B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>FirstName</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Happiest Minds</t>
   </si>
   <si>
-    <t>abc@gmail.com</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -79,22 +76,16 @@
     <t>Ranjeet</t>
   </si>
   <si>
-    <t>def@gmail.com</t>
-  </si>
-  <si>
-    <t>ghi@gmail.com</t>
-  </si>
-  <si>
-    <t>jkl@gmail.com</t>
-  </si>
-  <si>
-    <t>mno@gmail.com</t>
-  </si>
-  <si>
     <t>Senior Test Engineer</t>
   </si>
   <si>
     <t>Trainee Software Engineer</t>
+  </si>
+  <si>
+    <t>9876543210</t>
+  </si>
+  <si>
+    <t>Prashant.Chandra@ascendlearning.com</t>
   </si>
 </sst>
 </file>
@@ -162,7 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -174,6 +165,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -460,7 +454,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +463,7 @@
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -501,108 +495,100 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1">
-        <v>9876543210</v>
+        <v>21</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="1">
-        <v>9876543210</v>
+        <v>21</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="F4" s="1">
-        <v>9876543210</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="1">
-        <v>9876543210</v>
+      <c r="F5" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="1">
-        <v>9876543210</v>
+        <v>21</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{2ADB4267-2839-4A7A-B72C-B8A9343E54CB}"/>
-    <hyperlink ref="E3:E6" r:id="rId2" display="abc@gmail.com" xr:uid="{71120803-2E60-4BC7-9079-74243226C419}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{B7E39E13-712E-40FC-9EC8-EEAFF6B2F904}"/>
-    <hyperlink ref="E4" r:id="rId4" xr:uid="{FEDC7A29-6DAE-4FAE-A73B-3202BF75A69F}"/>
-    <hyperlink ref="E5" r:id="rId5" xr:uid="{31F11E16-F36E-4AF8-A49C-BB16ECCAC695}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{51C208E2-BCB5-4D86-A410-9416A17204DB}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added New Code Excel
</commit_message>
<xml_diff>
--- a/src/main/resources/ContactUsData.xlsx
+++ b/src/main/resources/ContactUsData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642C869B-A766-4515-8AB6-FFA0E2F9773B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30732303-FB01-44C2-98FA-BD10DAD9EC2A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,9 +55,6 @@
     <t>Rajesh</t>
   </si>
   <si>
-    <t>Prajatka</t>
-  </si>
-  <si>
     <t>Suryawanshi</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>Prashant.Chandra@ascendlearning.com</t>
+  </si>
+  <si>
+    <t>Prajakta</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,16 +495,16 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -515,76 +515,76 @@
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Code Excel Utils
</commit_message>
<xml_diff>
--- a/src/main/resources/ContactUsData.xlsx
+++ b/src/main/resources/ContactUsData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30732303-FB01-44C2-98FA-BD10DAD9EC2A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D08055-F530-47FB-8216-14AB43D3EC3C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,9 +453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>